<commit_message>
Ultimas alterações necessarias feitas - Troca total do banco de SQLite para SQLachemy
</commit_message>
<xml_diff>
--- a/FrontEnd/public/ArquivoDeExemplo.xlsx
+++ b/FrontEnd/public/ArquivoDeExemplo.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20408"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ct67ca\Desktop\FdT\ArquivosXML\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\51954963823\Desktop\Fdt-New\FrontEnd\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{800668ED-84A2-4D28-92A6-B473E3EEDC5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68309C4C-2C8C-4307-A2A5-74C3AAE536CC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F695E29C-55FD-4FA6-A190-7897CD78A2B6}"/>
   </bookViews>
@@ -20,56 +20,55 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
-  <si>
-    <t>Nome</t>
-  </si>
-  <si>
-    <t>EDV</t>
-  </si>
-  <si>
-    <t>Trilha</t>
-  </si>
-  <si>
-    <t>Gestor</t>
-  </si>
-  <si>
-    <t>EmailGestor</t>
-  </si>
-  <si>
-    <t>NomeGestorExempo</t>
-  </si>
-  <si>
-    <t>NomeColaboradorExemplo</t>
-  </si>
-  <si>
-    <t>TrilhaDoColaborador</t>
-  </si>
-  <si>
-    <t>emaildogestorexemplo@br.bosch.com</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
+  <si>
+    <t>nome</t>
+  </si>
+  <si>
+    <t>edv</t>
+  </si>
+  <si>
+    <t>trilha</t>
+  </si>
+  <si>
+    <t>gestor</t>
+  </si>
+  <si>
+    <t>gestor_email</t>
+  </si>
+  <si>
+    <t>Lucas</t>
+  </si>
+  <si>
+    <t>Lider</t>
+  </si>
+  <si>
+    <t>Henrique Dona</t>
+  </si>
+  <si>
+    <t>dona@br.bosch.com</t>
+  </si>
+  <si>
+    <t>Giovana</t>
+  </si>
+  <si>
+    <t>Qualidade</t>
+  </si>
+  <si>
+    <t>ESSA TABELA SERVE APENAS DE EXEMPLO, POR FAVOR SIGA O PADRÃO DELA 
+(AS TRILHAS DEVEM TER A PRIMEIRA LETRA EM MAIÚSCULO, EDV DEVE TER EXATOS 8 NÚMEROS ASSIM COMO NO CRACHA)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -85,13 +84,26 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -107,13 +119,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -430,10 +451,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44B35EA4-16CE-43B1-8CDB-704B2D6F17A1}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection sqref="A1:E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -446,44 +467,82 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
+      <c r="A1" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
       <c r="F1" s="1"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="4"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="1">
+        <v>12345678</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="1">
-        <v>92909290</v>
-      </c>
-      <c r="C2" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" s="2" t="s">
+      <c r="E4" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="3">
+        <v>87654321</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>8</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:E2"/>
+  </mergeCells>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" xr:uid="{DE541762-CE8F-4AF3-AA49-707D01583C28}"/>
+    <hyperlink ref="E4" r:id="rId1" xr:uid="{DE541762-CE8F-4AF3-AA49-707D01583C28}"/>
+    <hyperlink ref="E5" r:id="rId2" xr:uid="{8C7F57BC-3652-4CB7-85A3-71F7CCD5EDDD}"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>